<commit_message>
adds section about Verallgemeinbarkeit and needed document, updates tables
</commit_message>
<xml_diff>
--- a/documents/04-Analyse.xlsx
+++ b/documents/04-Analyse.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hohenberg/project/Masterthesis/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7831BDBB-8AD7-A84D-8C4B-7288FBE06C38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A0E9F3-5896-834C-84C3-3152040F5A4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{542D3738-8151-B74A-991A-6C4FC1990955}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19340" xr2:uid="{542D3738-8151-B74A-991A-6C4FC1990955}"/>
   </bookViews>
   <sheets>
     <sheet name="by paper" sheetId="2" r:id="rId1"/>
     <sheet name="summary" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="230">
   <si>
     <t>Aufteilung in internal, external und construct validity</t>
   </si>
@@ -565,9 +565,6 @@
     <t>Programmiersprachen</t>
   </si>
   <si>
-    <t>industrielle Teams</t>
-  </si>
-  <si>
     <t>Crowdtesting Platform</t>
   </si>
   <si>
@@ -661,9 +658,6 @@
     <t>other applications and grammar</t>
   </si>
   <si>
-    <t>large variety of applications and invalid inputs</t>
-  </si>
-  <si>
     <t>Kontext (S: Conclusion, P: Future Work)</t>
   </si>
   <si>
@@ -776,13 +770,85 @@
   </si>
   <si>
     <t>Zweck</t>
+  </si>
+  <si>
+    <t>Verweis auf future work</t>
+  </si>
+  <si>
+    <t>selection of apps</t>
+  </si>
+  <si>
+    <t>active analyzer and real world programs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> web testing, computer vision and information retrieval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use case mining, crowd-sourced use cases acquisition, and model </t>
+  </si>
+  <si>
+    <t>checking combos (ML applications)</t>
+  </si>
+  <si>
+    <t>X + Conclusion Validity - Construct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X  </t>
+  </si>
+  <si>
+    <t>OSS datasets with Puppet scripts</t>
+  </si>
+  <si>
+    <t>Kontexte (Z: Details S: Threats to Validity)</t>
+  </si>
+  <si>
+    <t>Kontexte (Z: Details S: Future Work)</t>
+  </si>
+  <si>
+    <t>across languages</t>
+  </si>
+  <si>
+    <t>new analysis</t>
+  </si>
+  <si>
+    <t>Android apps</t>
+  </si>
+  <si>
+    <t>Threats nicht vorhanden, aber</t>
+  </si>
+  <si>
+    <t>Limitations: 4</t>
+  </si>
+  <si>
+    <t>Future Work: 4</t>
+  </si>
+  <si>
+    <t>Limitations + Future Work: 2</t>
+  </si>
+  <si>
+    <t>Threats vorhanden</t>
+  </si>
+  <si>
+    <t>Limitations + Future Work: 6</t>
+  </si>
+  <si>
+    <t>Future Work: 12</t>
+  </si>
+  <si>
+    <t>Limitations: 3</t>
+  </si>
+  <si>
+    <t>Kontexte bgzl Verallgemeinbarkeit in ___ Paper gefunden</t>
+  </si>
+  <si>
+    <t>Entwickler, industrielle Teams</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -810,17 +876,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -941,7 +1014,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -986,7 +1059,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1024,6 +1097,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1395,9 +1470,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493611EB-B36F-BC49-9EE1-00D6FD60C398}">
   <dimension ref="A1:BH102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="137" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AB28" sqref="AB28:AB37"/>
+    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1599,7 +1674,7 @@
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
       <c r="G5" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H5" s="14" t="s">
         <v>18</v>
@@ -1620,11 +1695,11 @@
         <v>18</v>
       </c>
       <c r="N5" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O5">
-        <f>COUNTA(B5:N5)-2</f>
-        <v>9</v>
+        <f>COUNTA(B5:N5)-1</f>
+        <v>10</v>
       </c>
       <c r="Y5" s="4"/>
       <c r="Z5" s="3"/>
@@ -1829,14 +1904,14 @@
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J11" s="27"/>
       <c r="K11" s="11"/>
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>
       <c r="N11" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O11">
         <f t="shared" si="0"/>
@@ -1912,14 +1987,14 @@
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I13" s="27"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
       <c r="M13" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N13" s="8"/>
       <c r="O13">
@@ -1988,7 +2063,7 @@
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I15" s="27"/>
       <c r="J15" s="8"/>
@@ -2127,36 +2202,36 @@
     <row r="19" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A19" s="27"/>
       <c r="B19" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
       <c r="E19" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
       <c r="H19" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J19" s="16"/>
       <c r="K19" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L19" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M19" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N19" s="22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O19" s="29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="P19" s="16"/>
       <c r="Q19" s="16"/>
@@ -2176,7 +2251,7 @@
     <row r="20" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A20" s="27"/>
       <c r="B20" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
@@ -2186,23 +2261,23 @@
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
       <c r="H20" s="16" t="s">
-        <v>137</v>
+        <v>229</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J20" s="16"/>
       <c r="K20" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L20" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="M20" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="M20" s="22" t="s">
+      <c r="N20" s="22" t="s">
         <v>143</v>
-      </c>
-      <c r="N20" s="22" t="s">
-        <v>144</v>
       </c>
       <c r="O20">
         <f t="shared" ref="O20" si="1">COUNTA(B20:N20)</f>
@@ -2226,7 +2301,7 @@
     <row r="21" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A21" s="27"/>
       <c r="B21" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C21" s="16"/>
       <c r="D21" s="16" t="s">
@@ -2239,7 +2314,7 @@
       <c r="I21" s="16"/>
       <c r="J21" s="16"/>
       <c r="K21" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L21" s="16"/>
       <c r="M21" s="16"/>
@@ -3658,46 +3733,46 @@
     </row>
     <row r="42" spans="1:60" x14ac:dyDescent="0.2">
       <c r="AA42" s="29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AF42" s="2"/>
     </row>
     <row r="43" spans="1:60" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
+        <v>162</v>
+      </c>
+      <c r="C43" t="s">
         <v>163</v>
       </c>
-      <c r="C43" t="s">
-        <v>164</v>
-      </c>
       <c r="F43" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H43" t="s">
+        <v>151</v>
+      </c>
+      <c r="J43" t="s">
         <v>152</v>
       </c>
-      <c r="J43" t="s">
-        <v>153</v>
-      </c>
       <c r="L43" t="s">
+        <v>168</v>
+      </c>
+      <c r="N43" t="s">
+        <v>169</v>
+      </c>
+      <c r="R43" t="s">
+        <v>163</v>
+      </c>
+      <c r="V43" t="s">
         <v>170</v>
       </c>
-      <c r="N43" t="s">
-        <v>171</v>
-      </c>
-      <c r="R43" t="s">
-        <v>164</v>
-      </c>
-      <c r="V43" t="s">
+      <c r="X43" t="s">
         <v>172</v>
       </c>
-      <c r="X43" t="s">
+      <c r="Y43" t="s">
+        <v>173</v>
+      </c>
+      <c r="Z43" t="s">
         <v>174</v>
-      </c>
-      <c r="Y43" t="s">
-        <v>175</v>
-      </c>
-      <c r="Z43" t="s">
-        <v>176</v>
       </c>
       <c r="AA43" s="30">
         <f>COUNTA(B43:Z43)</f>
@@ -3716,13 +3791,13 @@
         <v>25</v>
       </c>
       <c r="H44" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I44" t="s">
         <v>15</v>
       </c>
       <c r="J44" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K44" t="s">
         <v>15</v>
@@ -3756,9 +3831,6 @@
       </c>
       <c r="F45" t="s">
         <v>28</v>
-      </c>
-      <c r="J45" t="s">
-        <v>169</v>
       </c>
       <c r="K45" t="s">
         <v>15</v>
@@ -3812,13 +3884,13 @@
     </row>
     <row r="47" spans="1:60" x14ac:dyDescent="0.2">
       <c r="F47" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M47" t="s">
         <v>15</v>
       </c>
       <c r="X47" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="Y47" t="s">
         <v>15</v>
@@ -3916,13 +3988,17 @@
       <c r="C55" s="25"/>
       <c r="D55" s="25"/>
       <c r="E55" s="25"/>
-      <c r="F55" s="25"/>
+      <c r="F55" s="24" t="s">
+        <v>212</v>
+      </c>
       <c r="G55" s="24" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H55" s="25"/>
       <c r="I55" s="25"/>
-      <c r="J55" s="25"/>
+      <c r="J55" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="K55" s="8"/>
       <c r="L55" s="8"/>
       <c r="M55" s="8"/>
@@ -3941,7 +4017,7 @@
       </c>
       <c r="S55">
         <f>COUNTA(B55:R55)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="W55" s="16"/>
       <c r="X55" s="34"/>
@@ -3953,12 +4029,16 @@
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="25"/>
-      <c r="D56" s="25"/>
+      <c r="D56" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="E56" s="25"/>
       <c r="F56" s="25"/>
       <c r="G56" s="24"/>
       <c r="H56" s="25"/>
-      <c r="I56" s="25"/>
+      <c r="I56" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="J56" s="25"/>
       <c r="K56" s="8" t="s">
         <v>18</v>
@@ -3972,7 +4052,7 @@
       <c r="R56" s="8"/>
       <c r="S56">
         <f>COUNTA(B56:R56)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W56" s="16"/>
       <c r="X56" s="35"/>
@@ -3983,7 +4063,9 @@
         <v>2</v>
       </c>
       <c r="B57" s="8"/>
-      <c r="C57" s="25"/>
+      <c r="C57" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="D57" s="25"/>
       <c r="E57" s="25"/>
       <c r="F57" s="25"/>
@@ -4001,7 +4083,7 @@
       <c r="R57" s="8"/>
       <c r="S57">
         <f t="shared" ref="S57:S70" si="3">COUNTA(B57:R57)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W57" s="16"/>
       <c r="X57" s="34"/>
@@ -4014,16 +4096,26 @@
       <c r="B58" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="C58" s="41"/>
-      <c r="D58" s="41"/>
+      <c r="C58" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58" s="41" t="s">
+        <v>18</v>
+      </c>
       <c r="E58" s="41"/>
-      <c r="F58" s="41"/>
+      <c r="F58" s="41" t="s">
+        <v>213</v>
+      </c>
       <c r="G58" s="42" t="s">
         <v>18</v>
       </c>
       <c r="H58" s="41"/>
-      <c r="I58" s="41"/>
-      <c r="J58" s="41"/>
+      <c r="I58" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="J58" s="41" t="s">
+        <v>18</v>
+      </c>
       <c r="K58" s="14" t="s">
         <v>18</v>
       </c>
@@ -4046,7 +4138,7 @@
       </c>
       <c r="S58" s="15">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="W58" s="16"/>
       <c r="X58" s="35"/>
@@ -4059,10 +4151,14 @@
       <c r="B59" s="11"/>
       <c r="C59" s="19"/>
       <c r="D59" s="19"/>
-      <c r="E59" s="19"/>
+      <c r="E59" s="19" t="s">
+        <v>18</v>
+      </c>
       <c r="F59" s="19"/>
       <c r="G59" s="43"/>
-      <c r="H59" s="19"/>
+      <c r="H59" s="19" t="s">
+        <v>18</v>
+      </c>
       <c r="I59" s="19"/>
       <c r="J59" s="19"/>
       <c r="K59" s="11"/>
@@ -4079,7 +4175,7 @@
       <c r="R59" s="11"/>
       <c r="S59" s="18">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="W59" s="16"/>
       <c r="X59" s="34"/>
@@ -4090,7 +4186,9 @@
         <v>3</v>
       </c>
       <c r="B60" s="8"/>
-      <c r="C60" s="25"/>
+      <c r="C60" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="D60" s="25"/>
       <c r="E60" s="25"/>
       <c r="F60" s="25"/>
@@ -4110,7 +4208,7 @@
       <c r="R60" s="8"/>
       <c r="S60">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W60" s="16"/>
       <c r="X60" s="3"/>
@@ -4121,8 +4219,12 @@
         <v>4</v>
       </c>
       <c r="B61" s="8"/>
-      <c r="C61" s="25"/>
-      <c r="D61" s="25"/>
+      <c r="C61" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D61" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="E61" s="25"/>
       <c r="F61" s="25"/>
       <c r="G61" s="24"/>
@@ -4147,7 +4249,7 @@
       <c r="R61" s="8"/>
       <c r="S61">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="W61" s="16"/>
       <c r="X61" s="3"/>
@@ -4190,12 +4292,16 @@
       </c>
       <c r="B63" s="8"/>
       <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
+      <c r="D63" s="25" t="s">
+        <v>206</v>
+      </c>
       <c r="E63" s="25"/>
       <c r="F63" s="25"/>
       <c r="G63" s="24"/>
       <c r="H63" s="25"/>
-      <c r="I63" s="25"/>
+      <c r="I63" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="J63" s="25"/>
       <c r="K63" s="8"/>
       <c r="L63" s="8"/>
@@ -4209,7 +4315,7 @@
       </c>
       <c r="S63" s="16">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W63" s="16"/>
       <c r="X63" s="34"/>
@@ -4220,35 +4326,41 @@
         <v>22</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C64" s="19"/>
       <c r="D64" s="19"/>
-      <c r="E64" s="19"/>
+      <c r="E64" s="19" t="s">
+        <v>80</v>
+      </c>
       <c r="F64" s="19"/>
       <c r="G64" s="43"/>
-      <c r="H64" s="19"/>
+      <c r="H64" s="19" t="s">
+        <v>218</v>
+      </c>
       <c r="I64" s="19"/>
-      <c r="J64" s="19"/>
+      <c r="J64" s="19" t="s">
+        <v>155</v>
+      </c>
       <c r="K64" s="11"/>
       <c r="L64" s="11" t="s">
         <v>80</v>
       </c>
       <c r="M64" s="11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="N64" s="11" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="O64" s="11"/>
       <c r="P64" s="11"/>
       <c r="Q64" s="11"/>
       <c r="R64" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="S64" s="18">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="W64" s="16"/>
       <c r="X64" s="34"/>
@@ -4292,8 +4404,12 @@
         <v>5</v>
       </c>
       <c r="B66" s="8"/>
-      <c r="C66" s="25"/>
-      <c r="D66" s="25"/>
+      <c r="C66" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D66" s="25" t="s">
+        <v>207</v>
+      </c>
       <c r="E66" s="25"/>
       <c r="F66" s="25"/>
       <c r="G66" s="24"/>
@@ -4304,17 +4420,17 @@
       <c r="L66" s="8"/>
       <c r="M66" s="8"/>
       <c r="N66" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="O66" s="8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="P66" s="8"/>
       <c r="Q66" s="8"/>
       <c r="R66" s="8"/>
       <c r="S66">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="W66" s="16"/>
       <c r="X66" s="34"/>
@@ -4334,7 +4450,9 @@
       </c>
       <c r="H67" s="25"/>
       <c r="I67" s="25"/>
-      <c r="J67" s="25"/>
+      <c r="J67" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="K67" s="8"/>
       <c r="L67" s="8"/>
       <c r="M67" s="8"/>
@@ -4345,7 +4463,7 @@
       <c r="R67" s="8"/>
       <c r="S67">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W67" s="16"/>
       <c r="X67" s="34"/>
@@ -4356,7 +4474,9 @@
         <v>26</v>
       </c>
       <c r="B68" s="8"/>
-      <c r="C68" s="25"/>
+      <c r="C68" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="D68" s="25"/>
       <c r="E68" s="25"/>
       <c r="F68" s="25"/>
@@ -4365,20 +4485,20 @@
       <c r="I68" s="25"/>
       <c r="J68" s="25"/>
       <c r="K68" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L68" s="8"/>
       <c r="M68" s="8"/>
       <c r="N68" s="8"/>
       <c r="O68" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="P68" s="8"/>
       <c r="Q68" s="8"/>
       <c r="R68" s="8"/>
       <c r="S68">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W68" s="16"/>
       <c r="X68" s="16"/>
@@ -4389,7 +4509,9 @@
         <v>38</v>
       </c>
       <c r="B69" s="8"/>
-      <c r="C69" s="25"/>
+      <c r="C69" s="25" t="s">
+        <v>18</v>
+      </c>
       <c r="D69" s="25"/>
       <c r="E69" s="25"/>
       <c r="F69" s="25"/>
@@ -4411,7 +4533,7 @@
       <c r="R69" s="8"/>
       <c r="S69">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:27" x14ac:dyDescent="0.2">
@@ -4442,139 +4564,150 @@
     </row>
     <row r="72" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
-        <v>153</v>
+        <v>152</v>
+      </c>
+      <c r="E72" t="s">
+        <v>151</v>
+      </c>
+      <c r="F72" t="s">
+        <v>152</v>
       </c>
       <c r="G72" t="s">
+        <v>151</v>
+      </c>
+      <c r="I72" t="s">
         <v>152</v>
       </c>
       <c r="L72" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="N72" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R72" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S72" s="29" t="s">
-        <v>145</v>
-      </c>
-      <c r="V72" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="W72" s="7"/>
-      <c r="X72" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="Y72" s="2"/>
-      <c r="Z72" s="2"/>
-      <c r="AA72" s="2"/>
+        <v>144</v>
+      </c>
+      <c r="V72" s="4"/>
+      <c r="W72" s="3"/>
+      <c r="X72" s="4"/>
+      <c r="Y72" s="4"/>
+      <c r="Z72" s="4"/>
+      <c r="AA72" s="4"/>
     </row>
     <row r="73" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
-        <v>184</v>
+        <v>182</v>
+      </c>
+      <c r="C73" s="46" t="s">
+        <v>216</v>
+      </c>
+      <c r="D73" s="46" t="s">
+        <v>215</v>
+      </c>
+      <c r="E73" t="s">
+        <v>208</v>
+      </c>
+      <c r="F73" t="s">
+        <v>214</v>
       </c>
       <c r="G73" t="s">
+        <v>186</v>
+      </c>
+      <c r="I73" t="s">
+        <v>219</v>
+      </c>
+      <c r="L73" t="s">
         <v>188</v>
-      </c>
-      <c r="L73" t="s">
-        <v>190</v>
       </c>
       <c r="M73" t="s">
         <v>15</v>
       </c>
       <c r="N73" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="R73" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="S73">
         <f t="shared" ref="S73" si="4">COUNTA(B73:R73)</f>
-        <v>6</v>
-      </c>
-      <c r="V73" s="33"/>
-      <c r="W73" s="40"/>
-      <c r="X73" s="33" t="s">
-        <v>180</v>
-      </c>
-      <c r="Y73" s="33" t="s">
-        <v>205</v>
-      </c>
-      <c r="Z73" s="33" t="s">
-        <v>206</v>
-      </c>
-      <c r="AA73" s="33" t="s">
-        <v>181</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="V73" s="4"/>
+      <c r="W73" s="3"/>
+      <c r="X73" s="4"/>
+      <c r="Y73" s="4"/>
+      <c r="Z73" s="4"/>
+      <c r="AA73" s="4"/>
     </row>
     <row r="74" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="C74" s="46" t="s">
+        <v>210</v>
+      </c>
+      <c r="D74" s="46" t="s">
+        <v>209</v>
+      </c>
+      <c r="F74" t="s">
+        <v>217</v>
+      </c>
       <c r="L74" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="M74" t="s">
         <v>15</v>
       </c>
       <c r="N74" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="R74" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="S74" t="s">
         <v>15</v>
       </c>
-      <c r="V74" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="W74" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="X74" s="2">
-        <v>3</v>
-      </c>
-      <c r="Y74" s="2"/>
-      <c r="Z74" s="2"/>
-      <c r="AA74" s="2"/>
+      <c r="V74" s="4"/>
+      <c r="W74" s="3"/>
+      <c r="X74" s="4"/>
+      <c r="Y74" s="4"/>
+      <c r="Z74" s="4"/>
+      <c r="AA74" s="4"/>
     </row>
     <row r="75" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
-        <v>152</v>
-      </c>
-      <c r="V75" s="2"/>
-      <c r="W75" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="X75" s="2"/>
-      <c r="Y75" s="2"/>
-      <c r="Z75" s="2"/>
-      <c r="AA75" s="2"/>
+        <v>151</v>
+      </c>
+      <c r="C75" s="46" t="s">
+        <v>211</v>
+      </c>
+      <c r="D75" s="46"/>
+      <c r="V75" s="4"/>
+      <c r="W75" s="3"/>
+      <c r="X75" s="4"/>
+      <c r="Y75" s="4"/>
+      <c r="Z75" s="4"/>
+      <c r="AA75" s="4"/>
     </row>
     <row r="76" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
-        <v>185</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="C76" s="46"/>
+      <c r="D76" s="46"/>
       <c r="I76" s="16"/>
       <c r="J76" s="16"/>
       <c r="K76" s="16"/>
       <c r="L76" s="16"/>
       <c r="R76" t="s">
-        <v>202</v>
-      </c>
-      <c r="V76" s="2"/>
-      <c r="W76" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="X76" s="2">
-        <v>2</v>
-      </c>
-      <c r="Y76" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z76" s="2">
-        <v>1</v>
-      </c>
-      <c r="AA76" s="2"/>
+        <v>200</v>
+      </c>
+      <c r="V76" s="4"/>
+      <c r="W76" s="3"/>
+      <c r="X76" s="4"/>
+      <c r="Y76" s="4"/>
+      <c r="Z76" s="4"/>
+      <c r="AA76" s="4"/>
     </row>
     <row r="77" spans="1:27" x14ac:dyDescent="0.2">
       <c r="I77" s="34"/>
@@ -4582,16 +4715,14 @@
       <c r="K77" s="16"/>
       <c r="L77" s="16"/>
       <c r="R77" t="s">
-        <v>203</v>
-      </c>
-      <c r="V77" s="2"/>
-      <c r="W77" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="X77" s="2"/>
-      <c r="Y77" s="2"/>
-      <c r="Z77" s="2"/>
-      <c r="AA77" s="2"/>
+        <v>201</v>
+      </c>
+      <c r="V77" s="4"/>
+      <c r="W77" s="3"/>
+      <c r="X77" s="4"/>
+      <c r="Y77" s="4"/>
+      <c r="Z77" s="4"/>
+      <c r="AA77" s="4"/>
     </row>
     <row r="78" spans="1:27" x14ac:dyDescent="0.2">
       <c r="I78" s="34"/>
@@ -4599,8 +4730,14 @@
       <c r="K78" s="16"/>
       <c r="L78" s="16"/>
       <c r="R78" t="s">
-        <v>204</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="V78" s="16"/>
+      <c r="W78" s="16"/>
+      <c r="X78" s="16"/>
+      <c r="Y78" s="16"/>
+      <c r="Z78" s="16"/>
+      <c r="AA78" s="16"/>
     </row>
     <row r="79" spans="1:27" x14ac:dyDescent="0.2">
       <c r="I79" s="34"/>
@@ -4901,18 +5038,18 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F99" s="29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C100" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E100" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F100" s="30">
         <f t="shared" ref="F100" si="6">COUNTA(B100:E100)</f>
@@ -4944,6 +5081,7 @@
   </sheetData>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -4953,7 +5091,7 @@
   <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView zoomScale="137" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4982,7 +5120,7 @@
       </c>
       <c r="G1" s="7"/>
       <c r="H1" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K1" s="6"/>
     </row>
@@ -4992,21 +5130,21 @@
       </c>
       <c r="B2" s="1">
         <f>'by paper'!O2+'by paper'!AA25+'by paper'!S55+'by paper'!F82</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F2" s="33"/>
       <c r="G2" s="40"/>
       <c r="H2" s="33" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I2" s="33" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J2" s="33" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K2" s="38" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -5015,13 +5153,13 @@
       </c>
       <c r="B3" s="1">
         <f>'by paper'!O3+'by paper'!AA26+'by paper'!S56+'by paper'!F83</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>177</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>179</v>
       </c>
       <c r="H3" s="2">
         <v>6</v>
@@ -5038,7 +5176,11 @@
       </c>
       <c r="B4" s="1">
         <f>'by paper'!O4+'by paper'!AA27+'by paper'!S57+'by paper'!F84</f>
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="C4" s="2">
+        <f>B2+B3+B4</f>
+        <v>34</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="7" t="s">
@@ -5059,11 +5201,15 @@
       </c>
       <c r="B5" s="1">
         <f>'by paper'!O5+'by paper'!AA28+'by paper'!S58+'by paper'!F85</f>
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="C5" s="2">
+        <f>B5+B6</f>
+        <v>59</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H5" s="2">
         <v>1</v>
@@ -5080,7 +5226,10 @@
       </c>
       <c r="B6" s="1">
         <f>'by paper'!O6+'by paper'!AA29+'by paper'!S59+'by paper'!F86</f>
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>220</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="7" t="s">
@@ -5099,7 +5248,10 @@
       </c>
       <c r="B7" s="1">
         <f>'by paper'!O7+'by paper'!AA30+'by paper'!S60+'by paper'!F87</f>
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="D7" s="47" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -5108,14 +5260,17 @@
       </c>
       <c r="B8" s="1">
         <f>'by paper'!O8+'by paper'!AA31+'by paper'!S61+'by paper'!F88</f>
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="D8" s="47" t="s">
+        <v>222</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K8" s="6"/>
     </row>
@@ -5127,19 +5282,22 @@
         <f>'by paper'!O9+'by paper'!AA32+'by paper'!S62+'by paper'!F89</f>
         <v>3</v>
       </c>
+      <c r="D9" s="47" t="s">
+        <v>223</v>
+      </c>
       <c r="F9" s="33"/>
       <c r="G9" s="40"/>
       <c r="H9" s="33" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I9" s="33" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J9" s="33" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K9" s="38" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -5148,13 +5306,13 @@
       </c>
       <c r="B10" s="1">
         <f>'by paper'!O10+'by paper'!AA33+'by paper'!S63+'by paper'!F90</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F10" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>177</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>179</v>
       </c>
       <c r="H10" s="2">
         <v>1</v>
@@ -5176,7 +5334,10 @@
       </c>
       <c r="B11" s="1">
         <f>'by paper'!O11+'by paper'!AA34+'by paper'!S64+'by paper'!F91</f>
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>224</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="7" t="s">
@@ -5202,9 +5363,12 @@
         <f>'by paper'!O12+'by paper'!AA35+'by paper'!S65+'by paper'!F92</f>
         <v>8</v>
       </c>
+      <c r="D12" s="47" t="s">
+        <v>227</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H12" s="2">
         <v>2</v>
@@ -5227,7 +5391,10 @@
       </c>
       <c r="B13" s="1">
         <f>'by paper'!O13+'by paper'!AA36+'by paper'!S66+'by paper'!F93</f>
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="D13" s="47" t="s">
+        <v>226</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="7" t="s">
@@ -5248,7 +5415,10 @@
       </c>
       <c r="B14" s="1">
         <f>'by paper'!O14+'by paper'!AA37+'by paper'!S67+'by paper'!F94</f>
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D14" s="47" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -5257,14 +5427,14 @@
       </c>
       <c r="B15" s="1">
         <f>'by paper'!O15+'by paper'!AA38+'by paper'!S68+'by paper'!F95</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K15" s="6"/>
     </row>
@@ -5274,21 +5444,21 @@
       </c>
       <c r="B16" s="1">
         <f>'by paper'!O16+'by paper'!AA39+'by paper'!S69+'by paper'!F96</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F16" s="33"/>
       <c r="G16" s="40"/>
       <c r="H16" s="33" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I16" s="33" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J16" s="33" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K16" s="38" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -5300,18 +5470,18 @@
         <v>3</v>
       </c>
       <c r="F17" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G17" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="G17" s="7" t="s">
-        <v>179</v>
-      </c>
       <c r="H17" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K17" s="6"/>
       <c r="L17" s="2">
         <f>SUM(H17:K17)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -5333,14 +5503,18 @@
       </c>
       <c r="B19" s="1">
         <f>'by paper'!O20+'by paper'!AA43+'by paper'!S73+'by paper'!F100</f>
-        <v>29</v>
+        <v>34</v>
+      </c>
+      <c r="C19" s="1">
+        <f>B19/0.59</f>
+        <v>57.627118644067799</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H19" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I19" s="2">
         <v>1</v>
@@ -5351,10 +5525,21 @@
       <c r="K19" s="6"/>
       <c r="L19" s="2">
         <f>SUM(H19:K19)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="39" t="s">
+        <v>228</v>
+      </c>
+      <c r="B20" s="1">
+        <f>B19-9</f>
+        <v>25</v>
+      </c>
+      <c r="C20" s="1">
+        <f>B20/0.59</f>
+        <v>42.372881355932208</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="7" t="s">
         <v>4</v>
@@ -5380,7 +5565,7 @@
       </c>
       <c r="G22" s="7"/>
       <c r="H22" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K22" s="6"/>
     </row>
@@ -5388,27 +5573,27 @@
       <c r="F23" s="33"/>
       <c r="G23" s="40"/>
       <c r="H23" s="33" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I23" s="33" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J23" s="33" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K23" s="38" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F24" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G24" s="7" t="s">
         <v>177</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>179</v>
       </c>
       <c r="H24" s="2">
         <v>2</v>
@@ -5421,7 +5606,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B25"/>
       <c r="C25" s="16"/>
@@ -5443,7 +5628,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B26"/>
       <c r="C26" s="16"/>
@@ -5451,7 +5636,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="2"/>
       <c r="G26" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H26" s="2"/>
       <c r="K26" s="6"/>
@@ -5462,7 +5647,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="7" t="s">
@@ -5477,52 +5662,52 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L28" s="2">
         <f>SUM(L3:L27)</f>
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E29" s="7"/>
       <c r="F29" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E30" s="40"/>
       <c r="F30" s="33" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H30" s="33" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I30" s="33" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J30" s="33" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K30" s="33" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E31" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F31" s="2">
         <f>H3+H10+H17+H24</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H31" s="35">
         <f>SUM(H3:H27)</f>
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="I31" s="35">
         <f>SUM(I3:I27)</f>
@@ -5538,7 +5723,7 @@
       </c>
       <c r="L31" s="2">
         <f>SUM(H31:K31)</f>
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
@@ -5559,11 +5744,11 @@
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F33" s="2">
         <f>H5+H12+H19+H26</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
@@ -5593,7 +5778,7 @@
       <c r="E35" s="16"/>
       <c r="F35" s="4">
         <f>SUM(F31:F34)</f>
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="4"/>
@@ -5865,6 +6050,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>